<commit_message>
Problematic queries dataset extension
</commit_message>
<xml_diff>
--- a/dataset/problematic_queries/spec_queries.xlsx
+++ b/dataset/problematic_queries/spec_queries.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\homeworks\NLP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\micha\homeworks\NLP\AgentToBeNamed\dataset\problematic_queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B917870-E151-44B0-A572-F83A2815FFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB38EE2-0A86-43CB-A492-46E4C692CB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A9DFE0ED-0099-4798-8085-7259020AA4A1}"/>
   </bookViews>
@@ -38,16 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
-    <t>task</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
     <t>Select rows where they consume more than 10.</t>
-  </si>
-  <si>
-    <t>table</t>
   </si>
   <si>
     <t>trans_data.xlsx</t>
@@ -71,13 +65,6 @@
     <t>Give me the cycle where elongation is the biggest on average based on length data</t>
   </si>
   <si>
-    <t xml:space="preserve">    # Calculate the biggest elongation based on acceleration data
-    biggest_elongation = df[df['length_mean']
-                         == df['length_mean'].min()]
-    # Return the cycle where elongation is the biggest on average
-    return biggest_elongation</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Give me the minimum of median forces in newtons measurment unit</t>
   </si>
   <si>
@@ -147,48 +134,16 @@
     <t>How many records were recorded by a VO id type?</t>
   </si>
   <si>
-    <t xml:space="preserve">    # Filter records with 'VO'
-    vo_records = df[df['vehicle_id'].str.contains(
-        'VO', case=False, na=False)]
-    # Count the number of records
-    num_records = len(vo_records)
-    # Return the number of records
-    return num_records</t>
-  </si>
-  <si>
     <t>Check if all first service dates are earlier or equal to end service dates. Return 1 for all correct, 0 for any incorrect.</t>
   </si>
   <si>
-    <t xml:space="preserve">    # Check if all first service dates are earlier or equal to end service dates
-    result = 1 if (df['first_service_date'] &lt;=
-                   df['last_service_date']).all() else 0
-    # Return the result
-    return result</t>
-  </si>
-  <si>
     <t>Check if all begin service dates are earlier to next service dates. Return 1 for all correct, 0 for any incorrect.</t>
   </si>
   <si>
-    <t xml:space="preserve">    # Check if all 'first_service_date' dates are earlier than 'next_service_date'
-    result = 1 if (df['first_service_date'] &lt;
-                   df['next_service_date']).all() else 0
-    # Return the result
-    return result</t>
-  </si>
-  <si>
     <t>Which model has the highest average positive fuel record?</t>
   </si>
   <si>
     <t>Which service type has the highest average cost of service?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    # Group the DataFrame by service type and calculate the average cost of service for each group
-    avg_cost_of_service_by_service_type = df.groupby('service_type')[
-        'cost_of_service'].mean()
-    # Find the service type with the highest average cost of service
-    service_type_highest_avg_cost_of_service = avg_cost_of_service_by_service_type.idxmax()
-    # Return the service type with the highest average cost of service
-    return service_type_highest_avg_cost_of_service</t>
   </si>
   <si>
     <t xml:space="preserve">    # Group the data by model and calculate the average positive fuel record
@@ -228,13 +183,6 @@
     <t>Count the total number of negative values across the current_mileage and initial_mileage columns.</t>
   </si>
   <si>
-    <t xml:space="preserve">    # Count the total number of negative values across the 'current_mileage' and 'initial_mileage' columns
-    count_negative_values = (df['current_mileage'] &lt; 0).sum(
-    ) + (df['initial_mileage'] &lt; 0).sum()
-    # Return the total count of negative values
-    return count_negative_values</t>
-  </si>
-  <si>
     <t>transactions_fin.xlsx</t>
   </si>
   <si>
@@ -268,22 +216,7 @@
     <t>i need top 15 percent of biggest differences in the eur czk rate and the usd czk rate of the one distinct transaction cycle</t>
   </si>
   <si>
-    <t xml:space="preserve">    # Calculate the difference in the eur czk rate and the usd czk rate
-    df['rate_difference'] = df['exchange_rate_eur_czk'] - \
-        df['exchange_rate_usd_czk']
-    # Calculate the top 15 percent of the biggest rate differences
-    top_percentile = df.nlargest(int(len(df) * 0.15), 'rate_difference')
-    return top_percentile</t>
-  </si>
-  <si>
     <t>rows with czk fees bigger or equal to 300, latency smaller than 475, where year is 2023 and batch status is Failed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    result = df[(df['Fees CZK'] &gt;= 300) &amp;
-                (df['Latency ms'] &lt; 475) &amp;
-                (df['Date'].str.contains('2023')) &amp;
-                (df['Batch Status'] == 'Failed')]
-    return result</t>
   </si>
   <si>
     <t>Give me the mean of paid amount in dollars by location</t>
@@ -328,16 +261,6 @@
     <t>Count rows for each currency type with date after January 2023</t>
   </si>
   <si>
-    <t xml:space="preserve">    # Convert Date to datetime
-    df['Date'] = pd.to_datetime(
-        df['Date'])
-    # Filter rows with Date after January 2023
-    df = df[df['Date'] &gt;= '2023-01-01']
-    # Count rows for each currency
-    count_per_currency = df['Currency'].value_counts()
-    return count_per_currency</t>
-  </si>
-  <si>
     <t>Find transactions where fees in eur were bigger than the average fee in usd and tag by 'eur_bigger' col</t>
   </si>
   <si>
@@ -352,11 +275,76 @@
     <t>Find the currency with the most significant difference in exchange_rate_eur_czk and exchange_rate_usd_czk for transactions that have a postal code greater than 60000.</t>
   </si>
   <si>
+    <t>table_name</t>
+  </si>
+  <si>
+    <t>user_query</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Calculate the biggest elongation based on acceleration data
+    biggest_elongation = df[df['length_mean'] == df['length_mean'].min()]
+    # Return the cycle where elongation is the biggest on average
+    return biggest_elongation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Filter records with 'VO'
+    vo_records = df[df['vehicle_id'].str.contains('VO', case=False, na=False)]
+    # Count the number of records
+    num_records = len(vo_records)
+    # Return the number of records
+    return num_records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Check if all first service dates are earlier or equal to end service dates
+    result = 1 if (df['first_service_date'] &lt;= df['last_service_date']).all() else 0
+    # Return the result
+    return result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Check if all 'first_service_date' dates are earlier than 'next_service_date'
+    result = 1 if (df['first_service_date'] &lt; df['next_service_date']).all() else 0
+    # Return the result
+    return result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Group the DataFrame by service type and calculate the average cost of service for each group
+    avg_cost_of_service_by_service_type = df.groupby('service_type')['cost_of_service'].mean()
+    # Find the service type with the highest average cost of service
+    service_type_highest_avg_cost_of_service = avg_cost_of_service_by_service_type.idxmax()
+    # Return the service type with the highest average cost of service
+    return service_type_highest_avg_cost_of_service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Count the total number of negative values across the 'current_mileage' and 'initial_mileage' columns
+    count_negative_values = (df['current_mileage'] &lt; 0).sum() + (df['initial_mileage'] &lt; 0).sum()
+    # Return the total count of negative values
+    return count_negative_values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Calculate the difference in the eur czk rate and the usd czk rate
+    df['rate_difference'] = df['exchange_rate_eur_czk'] - df['exchange_rate_usd_czk']
+    # Calculate the top 15 percent of the biggest rate differences
+    top_percentile = df.nlargest(int(len(df) * 0.15), 'rate_difference')
+    return top_percentile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    result = df[(df['Fees CZK'] &gt;= 300) &amp; (df['Latency ms'] &lt; 475) &amp; (df['Date'].str.contains('2023')) &amp; (df['Batch Status'] == 'Failed')]
+    return result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Convert Date to datetime
+    df['Date'] = pd.to_datetime(df['Date'])
+    # Filter rows with Date after January 2023
+    df = df[df['Date'] &gt;= '2023-01-01']
+    # Count rows for each currency
+    count_per_currency = df['Currency'].value_counts()
+    return count_per_currency</t>
+  </si>
+  <si>
     <t xml:space="preserve">    # Filter transactions with Postal Code greater than 60000
     filtered_df = df[df['Postal Code'] &gt; 60000]
     # Calculate the difference in exchange_rate_eur_czk and exchange_rate_usd_czk
-    filtered_df['rate_diff'] = filtered_df['exchange_rate_usd_czk'] - \
-        filtered_df['exchange_rate_eur_czk']
+    filtered_df['rate_diff'] = filtered_df['exchange_rate_usd_czk'] - filtered_df['exchange_rate_eur_czk']
     # Find the currency with the most significant difference
     result = filtered_df.loc[filtered_df['rate_diff'].idxmax()]['Currency']
     return result</t>
@@ -768,363 +756,363 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="104.85546875" customWidth="1"/>
-    <col min="3" max="3" width="60.5703125" customWidth="1"/>
+    <col min="3" max="3" width="123.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C25" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="27" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="28" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="29" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="30" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C31" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="1" t="s">
+    </row>
+    <row r="32" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" t="s">
-        <v>65</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>66</v>

</xml_diff>